<commit_message>
stresses and simulation modified
</commit_message>
<xml_diff>
--- a/project_stresses.xlsx
+++ b/project_stresses.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2021-2022 Fall\EE463\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre Çakmakyurdu\Documents\EE463-Static-Power-Conversion-1--Term-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C504D2-EFF4-4749-BEFA-6E7998F6589E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6030"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Rectifier Diode Reverse Voltage</t>
   </si>
@@ -44,29 +54,119 @@
     <t>MOSFET Current</t>
   </si>
   <si>
-    <t>Input current THD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D=0.1 </t>
+    <t>Output Average Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power </t>
+  </si>
+  <si>
+    <t>D = 0.1 - Startup ( Back emf = 0.1V)</t>
+  </si>
+  <si>
+    <t>25 A</t>
+  </si>
+  <si>
+    <t>21 A</t>
+  </si>
+  <si>
+    <t>(-) 242 V</t>
+  </si>
+  <si>
+    <t>246 V</t>
+  </si>
+  <si>
+    <t>15 A</t>
+  </si>
+  <si>
+    <t>Maximum Armature Current</t>
+  </si>
+  <si>
+    <t>22.4 A</t>
+  </si>
+  <si>
+    <t>23.45 V</t>
+  </si>
+  <si>
+    <t>514.7 W</t>
+  </si>
+  <si>
+    <t>D = 0.8 - Steady state ( Back emf = 220 V)</t>
+  </si>
+  <si>
+    <t>19 A</t>
+  </si>
+  <si>
+    <t>(-) 244 V</t>
+  </si>
+  <si>
+    <t>16 A</t>
+  </si>
+  <si>
+    <t>245 V</t>
+  </si>
+  <si>
+    <t>17 A</t>
+  </si>
+  <si>
+    <t>186 V</t>
+  </si>
+  <si>
+    <t>14.2 A</t>
+  </si>
+  <si>
+    <t>2500 W</t>
+  </si>
+  <si>
+    <t>Vin = 100 V  / f = 1kHz</t>
+  </si>
+  <si>
+    <t>Vin = 90 V / f = 10 kHz</t>
+  </si>
+  <si>
+    <t>D = 0.1 - Startup ( Back emf = 220 V)</t>
+  </si>
+  <si>
+    <t>19 A ( Note: 33 A spike)</t>
+  </si>
+  <si>
+    <t>(-) 220 V</t>
+  </si>
+  <si>
+    <t>220 V</t>
+  </si>
+  <si>
+    <t>18 A</t>
+  </si>
+  <si>
+    <t>(-) 217V</t>
+  </si>
+  <si>
+    <t>20 V</t>
+  </si>
+  <si>
+    <t>20 A</t>
+  </si>
+  <si>
+    <t>165.4 V</t>
+  </si>
+  <si>
+    <t>2807 W</t>
+  </si>
+  <si>
+    <t>23.4 A</t>
+  </si>
+  <si>
+    <t>(-) 217 V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -82,15 +182,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,35 +208,25 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+  <cellStyles count="2">
+    <cellStyle name="Başlık 2" xfId="1" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,76 +504,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>